<commit_message>
Create New Xlsx translate function (xlwings lib)
</commit_message>
<xml_diff>
--- a/test script/Test file for shape and rich text 2.xlsx
+++ b/test script/Test file for shape and rich text 2.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evan\Documents\GitHub\aiotranslator4\test script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{52EDDAFE-0BEB-4838-A7F9-F9950C0E74DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{22974695-F313-41B1-AEE7-8C0878F1AFE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29880" yWindow="1080" windowWidth="15330" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -756,7 +757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
@@ -775,4 +776,16 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A7F476-D959-4E04-88AD-0709B9E5F592}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>